<commit_message>
PowerShell integration with drag and drop capabilities
</commit_message>
<xml_diff>
--- a/misc/PR_form.xlsx
+++ b/misc/PR_form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Scripts\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09886364-DCA5-4ACE-8C9B-E5248740AC4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C5E453-C152-411D-B560-7F55C4017F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4920" yWindow="1770" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Purchase Order request form" sheetId="1" r:id="rId1"/>
@@ -465,13 +465,13 @@
     <t>each</t>
   </si>
   <si>
-    <t>BDI CANADA</t>
-  </si>
-  <si>
-    <t>Lubricators for trial test</t>
-  </si>
-  <si>
     <t>As per attached quotation</t>
+  </si>
+  <si>
+    <t>Acklands Grainger</t>
+  </si>
+  <si>
+    <t>Personal Tools</t>
   </si>
 </sst>
 </file>
@@ -2938,8 +2938,8 @@
   </sheetPr>
   <dimension ref="A1:AM80"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:I18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18:N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3142,7 +3142,7 @@
         <v>31</v>
       </c>
       <c r="H5" s="188">
-        <v>45138</v>
+        <v>45141</v>
       </c>
       <c r="I5" s="188"/>
       <c r="J5" s="188"/>
@@ -3229,7 +3229,7 @@
         <v>108</v>
       </c>
       <c r="C7" s="153" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D7" s="153"/>
       <c r="E7" s="153"/>
@@ -3695,7 +3695,7 @@
       <c r="B17" s="284"/>
       <c r="C17" s="285"/>
       <c r="D17" s="167" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E17" s="168"/>
       <c r="F17" s="168"/>
@@ -3709,13 +3709,13 @@
         <v>1</v>
       </c>
       <c r="L17" s="154">
-        <v>299</v>
+        <v>325</v>
       </c>
       <c r="M17" s="155"/>
       <c r="N17" s="156"/>
       <c r="O17" s="165">
         <f t="shared" ref="O17:O20" si="0">K17*L17</f>
-        <v>299</v>
+        <v>325</v>
       </c>
       <c r="P17" s="165"/>
       <c r="Q17" s="165"/>
@@ -3747,7 +3747,7 @@
       <c r="B18" s="190"/>
       <c r="C18" s="191"/>
       <c r="D18" s="170" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E18" s="171"/>
       <c r="F18" s="171"/>
@@ -4249,7 +4249,7 @@
       <c r="N29" s="141"/>
       <c r="O29" s="214">
         <f>SUM(O17:S28)</f>
-        <v>299</v>
+        <v>325</v>
       </c>
       <c r="P29" s="214"/>
       <c r="Q29" s="214"/>
@@ -4348,7 +4348,7 @@
       <c r="N31" s="259"/>
       <c r="O31" s="247">
         <f>0.13*(O29+O30)</f>
-        <v>38.870000000000005</v>
+        <v>42.25</v>
       </c>
       <c r="P31" s="248"/>
       <c r="Q31" s="248"/>
@@ -4437,7 +4437,7 @@
       <c r="N33" s="261"/>
       <c r="O33" s="244">
         <f>O29+O30+O31</f>
-        <v>337.87</v>
+        <v>367.25</v>
       </c>
       <c r="P33" s="245"/>
       <c r="Q33" s="245"/>

</xml_diff>

<commit_message>
Move scripts to bin folder and change paths on scripts
</commit_message>
<xml_diff>
--- a/misc/PR_form.xlsx
+++ b/misc/PR_form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Scripts\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C5E453-C152-411D-B560-7F55C4017F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630CBF49-F3CD-4DED-9679-E42F7560B97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4920" yWindow="1770" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -468,10 +468,10 @@
     <t>As per attached quotation</t>
   </si>
   <si>
-    <t>Acklands Grainger</t>
-  </si>
-  <si>
-    <t>Personal Tools</t>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Petro Canada Lubricants</t>
   </si>
 </sst>
 </file>
@@ -1899,15 +1899,61 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="170" fontId="11" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -1923,321 +1969,26 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="169" fontId="11" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="167" fontId="45" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -2325,6 +2076,14 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
@@ -2353,53 +2112,294 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="11" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="168" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2938,8 +2938,8 @@
   </sheetPr>
   <dimension ref="A1:AM80"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18:N18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2993,22 +2993,22 @@
     <row r="2" spans="1:39" s="1" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="112"/>
       <c r="F2" s="34"/>
-      <c r="G2" s="274" t="s">
+      <c r="G2" s="154" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="274"/>
-      <c r="I2" s="274"/>
-      <c r="J2" s="274"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+      <c r="J2" s="154"/>
       <c r="K2" s="34"/>
-      <c r="L2" s="278" t="s">
+      <c r="L2" s="158" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="279"/>
-      <c r="N2" s="279"/>
-      <c r="O2" s="279"/>
-      <c r="P2" s="279"/>
-      <c r="Q2" s="279"/>
-      <c r="R2" s="279"/>
+      <c r="M2" s="159"/>
+      <c r="N2" s="159"/>
+      <c r="O2" s="159"/>
+      <c r="P2" s="159"/>
+      <c r="Q2" s="159"/>
+      <c r="R2" s="159"/>
       <c r="S2" s="18"/>
       <c r="T2" s="112"/>
       <c r="U2" s="117"/>
@@ -3035,30 +3035,30 @@
     </row>
     <row r="3" spans="1:39" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="112"/>
-      <c r="B3" s="286" t="s">
+      <c r="B3" s="176" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="286"/>
-      <c r="D3" s="182" t="s">
+      <c r="C3" s="176"/>
+      <c r="D3" s="162" t="s">
         <v>105</v>
       </c>
-      <c r="E3" s="182"/>
-      <c r="F3" s="275"/>
-      <c r="G3" s="275"/>
-      <c r="H3" s="275"/>
-      <c r="I3" s="275"/>
-      <c r="J3" s="275"/>
-      <c r="K3" s="275"/>
+      <c r="E3" s="162"/>
+      <c r="F3" s="155"/>
+      <c r="G3" s="155"/>
+      <c r="H3" s="155"/>
+      <c r="I3" s="155"/>
+      <c r="J3" s="155"/>
+      <c r="K3" s="155"/>
       <c r="L3" s="109" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="176"/>
-      <c r="N3" s="176"/>
-      <c r="O3" s="176"/>
-      <c r="P3" s="176"/>
-      <c r="Q3" s="176"/>
-      <c r="R3" s="176"/>
-      <c r="S3" s="177"/>
+      <c r="M3" s="264"/>
+      <c r="N3" s="264"/>
+      <c r="O3" s="264"/>
+      <c r="P3" s="264"/>
+      <c r="Q3" s="264"/>
+      <c r="R3" s="264"/>
+      <c r="S3" s="265"/>
       <c r="T3" s="112"/>
       <c r="U3" s="117"/>
       <c r="V3" s="120" t="s">
@@ -3084,38 +3084,38 @@
     </row>
     <row r="4" spans="1:39" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="112"/>
-      <c r="B4" s="187" t="s">
+      <c r="B4" s="245" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="187"/>
-      <c r="D4" s="189" t="s">
+      <c r="C4" s="245"/>
+      <c r="D4" s="247" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="189"/>
-      <c r="F4" s="276" t="s">
+      <c r="E4" s="247"/>
+      <c r="F4" s="156" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="277"/>
-      <c r="H4" s="277"/>
-      <c r="I4" s="277"/>
-      <c r="J4" s="277"/>
-      <c r="K4" s="277"/>
+      <c r="G4" s="157"/>
+      <c r="H4" s="157"/>
+      <c r="I4" s="157"/>
+      <c r="J4" s="157"/>
+      <c r="K4" s="157"/>
       <c r="L4" s="21"/>
-      <c r="M4" s="178"/>
-      <c r="N4" s="178"/>
-      <c r="O4" s="178"/>
-      <c r="P4" s="178"/>
-      <c r="Q4" s="178"/>
-      <c r="R4" s="178"/>
-      <c r="S4" s="179"/>
+      <c r="M4" s="266"/>
+      <c r="N4" s="266"/>
+      <c r="O4" s="266"/>
+      <c r="P4" s="266"/>
+      <c r="Q4" s="266"/>
+      <c r="R4" s="266"/>
+      <c r="S4" s="267"/>
       <c r="T4" s="112"/>
       <c r="U4" s="117"/>
       <c r="V4" s="120" t="s">
         <v>68</v>
       </c>
-      <c r="W4" s="183"/>
-      <c r="X4" s="183"/>
-      <c r="Y4" s="183"/>
+      <c r="W4" s="244"/>
+      <c r="X4" s="244"/>
+      <c r="Y4" s="244"/>
       <c r="Z4" s="117"/>
       <c r="AA4" s="117"/>
       <c r="AB4" s="117"/>
@@ -3141,26 +3141,26 @@
       <c r="G5" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="188">
-        <v>45141</v>
-      </c>
-      <c r="I5" s="188"/>
-      <c r="J5" s="188"/>
+      <c r="H5" s="246">
+        <v>45142</v>
+      </c>
+      <c r="I5" s="246"/>
+      <c r="J5" s="246"/>
       <c r="K5" s="5"/>
       <c r="L5" s="20"/>
-      <c r="M5" s="180"/>
-      <c r="N5" s="180"/>
-      <c r="O5" s="180"/>
-      <c r="P5" s="180"/>
-      <c r="Q5" s="180"/>
-      <c r="R5" s="180"/>
+      <c r="M5" s="268"/>
+      <c r="N5" s="268"/>
+      <c r="O5" s="268"/>
+      <c r="P5" s="268"/>
+      <c r="Q5" s="268"/>
+      <c r="R5" s="268"/>
       <c r="S5" s="111"/>
       <c r="T5" s="112"/>
       <c r="U5" s="117"/>
       <c r="V5" s="120"/>
-      <c r="W5" s="183"/>
-      <c r="X5" s="183"/>
-      <c r="Y5" s="183"/>
+      <c r="W5" s="244"/>
+      <c r="X5" s="244"/>
+      <c r="Y5" s="244"/>
       <c r="Z5" s="117"/>
       <c r="AA5" s="117"/>
       <c r="AB5" s="117"/>
@@ -3178,13 +3178,13 @@
     </row>
     <row r="6" spans="1:39" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="112"/>
-      <c r="B6" s="203" t="s">
+      <c r="B6" s="258" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="203"/>
-      <c r="D6" s="203"/>
-      <c r="E6" s="203"/>
-      <c r="F6" s="204"/>
+      <c r="C6" s="258"/>
+      <c r="D6" s="258"/>
+      <c r="E6" s="258"/>
+      <c r="F6" s="166"/>
       <c r="G6" s="80" t="s">
         <v>25</v>
       </c>
@@ -3229,28 +3229,28 @@
         <v>108</v>
       </c>
       <c r="C7" s="153" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D7" s="153"/>
       <c r="E7" s="153"/>
       <c r="F7" s="16"/>
       <c r="G7" s="81"/>
-      <c r="H7" s="182" t="s">
+      <c r="H7" s="162" t="s">
         <v>109</v>
       </c>
-      <c r="I7" s="182"/>
-      <c r="J7" s="182"/>
+      <c r="I7" s="162"/>
+      <c r="J7" s="162"/>
       <c r="K7" s="5"/>
-      <c r="L7" s="184" t="s">
+      <c r="L7" s="270" t="s">
         <v>37</v>
       </c>
-      <c r="M7" s="184"/>
-      <c r="N7" s="184"/>
-      <c r="O7" s="184"/>
-      <c r="P7" s="184"/>
-      <c r="Q7" s="184"/>
-      <c r="R7" s="184"/>
-      <c r="S7" s="184"/>
+      <c r="M7" s="270"/>
+      <c r="N7" s="270"/>
+      <c r="O7" s="270"/>
+      <c r="P7" s="270"/>
+      <c r="Q7" s="270"/>
+      <c r="R7" s="270"/>
+      <c r="S7" s="270"/>
       <c r="T7" s="121"/>
       <c r="U7" s="122"/>
       <c r="V7" s="120" t="s">
@@ -3283,27 +3283,27 @@
       <c r="G8" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="280" t="s">
+      <c r="H8" s="163" t="s">
         <v>106</v>
       </c>
-      <c r="I8" s="280"/>
-      <c r="J8" s="280"/>
+      <c r="I8" s="163"/>
+      <c r="J8" s="163"/>
       <c r="K8" s="25"/>
-      <c r="L8" s="185"/>
-      <c r="M8" s="185"/>
-      <c r="N8" s="185"/>
-      <c r="O8" s="185"/>
-      <c r="P8" s="185"/>
-      <c r="Q8" s="185"/>
-      <c r="R8" s="185"/>
-      <c r="S8" s="185"/>
+      <c r="L8" s="271"/>
+      <c r="M8" s="271"/>
+      <c r="N8" s="271"/>
+      <c r="O8" s="271"/>
+      <c r="P8" s="271"/>
+      <c r="Q8" s="271"/>
+      <c r="R8" s="271"/>
+      <c r="S8" s="271"/>
       <c r="T8" s="121"/>
       <c r="U8" s="122"/>
       <c r="V8" s="120" t="s">
         <v>67</v>
       </c>
-      <c r="W8" s="183"/>
-      <c r="X8" s="183"/>
+      <c r="W8" s="244"/>
+      <c r="X8" s="244"/>
       <c r="Y8" s="120"/>
       <c r="Z8" s="122"/>
       <c r="AA8" s="122"/>
@@ -3325,9 +3325,9 @@
       <c r="B9" s="76" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="181"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="181"/>
+      <c r="C9" s="269"/>
+      <c r="D9" s="269"/>
+      <c r="E9" s="269"/>
       <c r="F9" s="32"/>
       <c r="G9" s="44" t="s">
         <v>5</v>
@@ -3347,8 +3347,8 @@
       <c r="T9" s="121"/>
       <c r="U9" s="122"/>
       <c r="V9" s="120"/>
-      <c r="W9" s="183"/>
-      <c r="X9" s="183"/>
+      <c r="W9" s="244"/>
+      <c r="X9" s="244"/>
       <c r="Y9" s="123"/>
       <c r="Z9" s="122"/>
       <c r="AA9" s="122"/>
@@ -3370,14 +3370,14 @@
       <c r="B10" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="186"/>
-      <c r="D10" s="186"/>
-      <c r="E10" s="186"/>
+      <c r="C10" s="272"/>
+      <c r="D10" s="272"/>
+      <c r="E10" s="272"/>
       <c r="F10" s="33"/>
-      <c r="G10" s="197"/>
-      <c r="H10" s="197"/>
-      <c r="I10" s="197"/>
-      <c r="J10" s="197"/>
+      <c r="G10" s="253"/>
+      <c r="H10" s="253"/>
+      <c r="I10" s="253"/>
+      <c r="J10" s="253"/>
       <c r="K10" s="25"/>
       <c r="L10" s="44" t="s">
         <v>18</v>
@@ -3394,8 +3394,8 @@
       <c r="V10" s="120" t="s">
         <v>69</v>
       </c>
-      <c r="W10" s="183"/>
-      <c r="X10" s="183"/>
+      <c r="W10" s="244"/>
+      <c r="X10" s="244"/>
       <c r="Y10" s="124"/>
       <c r="Z10" s="122"/>
       <c r="AA10" s="122"/>
@@ -3426,16 +3426,16 @@
       <c r="I11" s="23"/>
       <c r="J11" s="23"/>
       <c r="K11" s="25"/>
-      <c r="L11" s="205" t="s">
+      <c r="L11" s="175" t="s">
         <v>102</v>
       </c>
-      <c r="M11" s="205"/>
-      <c r="N11" s="205"/>
-      <c r="O11" s="205"/>
-      <c r="P11" s="205"/>
-      <c r="Q11" s="205"/>
-      <c r="R11" s="205"/>
-      <c r="S11" s="205"/>
+      <c r="M11" s="175"/>
+      <c r="N11" s="175"/>
+      <c r="O11" s="175"/>
+      <c r="P11" s="175"/>
+      <c r="Q11" s="175"/>
+      <c r="R11" s="175"/>
+      <c r="S11" s="175"/>
       <c r="T11" s="121"/>
       <c r="U11" s="122"/>
       <c r="V11" s="120"/>
@@ -3464,21 +3464,21 @@
       <c r="D12" s="31"/>
       <c r="E12" s="31"/>
       <c r="F12" s="24"/>
-      <c r="G12" s="283"/>
-      <c r="H12" s="283"/>
-      <c r="I12" s="283"/>
-      <c r="J12" s="283"/>
+      <c r="G12" s="167"/>
+      <c r="H12" s="167"/>
+      <c r="I12" s="167"/>
+      <c r="J12" s="167"/>
       <c r="K12" s="23"/>
-      <c r="L12" s="205" t="s">
+      <c r="L12" s="175" t="s">
         <v>100</v>
       </c>
-      <c r="M12" s="205"/>
-      <c r="N12" s="205"/>
-      <c r="O12" s="205"/>
-      <c r="P12" s="205"/>
-      <c r="Q12" s="205"/>
-      <c r="R12" s="205"/>
-      <c r="S12" s="205"/>
+      <c r="M12" s="175"/>
+      <c r="N12" s="175"/>
+      <c r="O12" s="175"/>
+      <c r="P12" s="175"/>
+      <c r="Q12" s="175"/>
+      <c r="R12" s="175"/>
+      <c r="S12" s="175"/>
       <c r="T12" s="112"/>
       <c r="U12" s="117"/>
       <c r="V12" s="120" t="s">
@@ -3504,12 +3504,12 @@
     </row>
     <row r="13" spans="1:39" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="112"/>
-      <c r="B13" s="282" t="s">
+      <c r="B13" s="165" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="282"/>
-      <c r="D13" s="282"/>
-      <c r="E13" s="204"/>
+      <c r="C13" s="165"/>
+      <c r="D13" s="165"/>
+      <c r="E13" s="166"/>
       <c r="F13" s="24"/>
       <c r="G13" s="44" t="s">
         <v>76</v>
@@ -3518,16 +3518,16 @@
       <c r="I13" s="23"/>
       <c r="J13" s="23"/>
       <c r="K13" s="23"/>
-      <c r="L13" s="205" t="s">
+      <c r="L13" s="175" t="s">
         <v>101</v>
       </c>
-      <c r="M13" s="205"/>
-      <c r="N13" s="205"/>
-      <c r="O13" s="205"/>
-      <c r="P13" s="205"/>
-      <c r="Q13" s="205"/>
-      <c r="R13" s="205"/>
-      <c r="S13" s="205"/>
+      <c r="M13" s="175"/>
+      <c r="N13" s="175"/>
+      <c r="O13" s="175"/>
+      <c r="P13" s="175"/>
+      <c r="Q13" s="175"/>
+      <c r="R13" s="175"/>
+      <c r="S13" s="175"/>
       <c r="T13" s="112"/>
       <c r="U13" s="117"/>
       <c r="V13" s="120" t="s">
@@ -3553,26 +3553,26 @@
     </row>
     <row r="14" spans="1:39" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="112"/>
-      <c r="B14" s="281"/>
-      <c r="C14" s="281"/>
-      <c r="D14" s="281"/>
+      <c r="B14" s="164"/>
+      <c r="C14" s="164"/>
+      <c r="D14" s="164"/>
       <c r="E14" s="60"/>
       <c r="F14" s="24"/>
-      <c r="G14" s="198"/>
-      <c r="H14" s="198"/>
-      <c r="I14" s="198"/>
-      <c r="J14" s="198"/>
+      <c r="G14" s="254"/>
+      <c r="H14" s="254"/>
+      <c r="I14" s="254"/>
+      <c r="J14" s="254"/>
       <c r="K14" s="23"/>
-      <c r="L14" s="205" t="s">
+      <c r="L14" s="175" t="s">
         <v>103</v>
       </c>
-      <c r="M14" s="205"/>
-      <c r="N14" s="205"/>
-      <c r="O14" s="205"/>
-      <c r="P14" s="205"/>
-      <c r="Q14" s="205"/>
-      <c r="R14" s="205"/>
-      <c r="S14" s="205"/>
+      <c r="M14" s="175"/>
+      <c r="N14" s="175"/>
+      <c r="O14" s="175"/>
+      <c r="P14" s="175"/>
+      <c r="Q14" s="175"/>
+      <c r="R14" s="175"/>
+      <c r="S14" s="175"/>
       <c r="T14" s="112"/>
       <c r="U14" s="117"/>
       <c r="V14" s="120" t="s">
@@ -3637,36 +3637,36 @@
     </row>
     <row r="16" spans="1:39" s="99" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="114"/>
-      <c r="B16" s="206" t="s">
+      <c r="B16" s="259" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="207"/>
-      <c r="D16" s="160" t="s">
+      <c r="C16" s="260"/>
+      <c r="D16" s="261" t="s">
         <v>0</v>
       </c>
-      <c r="E16" s="161"/>
-      <c r="F16" s="161"/>
-      <c r="G16" s="161"/>
-      <c r="H16" s="161"/>
-      <c r="I16" s="162"/>
+      <c r="E16" s="262"/>
+      <c r="F16" s="262"/>
+      <c r="G16" s="262"/>
+      <c r="H16" s="262"/>
+      <c r="I16" s="263"/>
       <c r="J16" s="139" t="s">
         <v>33</v>
       </c>
       <c r="K16" s="139" t="s">
         <v>19</v>
       </c>
-      <c r="L16" s="160" t="s">
+      <c r="L16" s="261" t="s">
         <v>1</v>
       </c>
-      <c r="M16" s="161"/>
-      <c r="N16" s="162"/>
-      <c r="O16" s="163" t="s">
+      <c r="M16" s="262"/>
+      <c r="N16" s="263"/>
+      <c r="O16" s="276" t="s">
         <v>2</v>
       </c>
-      <c r="P16" s="163"/>
-      <c r="Q16" s="163"/>
-      <c r="R16" s="163"/>
-      <c r="S16" s="164"/>
+      <c r="P16" s="276"/>
+      <c r="Q16" s="276"/>
+      <c r="R16" s="276"/>
+      <c r="S16" s="277"/>
       <c r="T16" s="125"/>
       <c r="U16" s="126"/>
       <c r="V16" s="120" t="s">
@@ -3692,35 +3692,35 @@
     </row>
     <row r="17" spans="1:39" s="3" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="115"/>
-      <c r="B17" s="284"/>
-      <c r="C17" s="285"/>
-      <c r="D17" s="167" t="s">
-        <v>114</v>
-      </c>
-      <c r="E17" s="168"/>
-      <c r="F17" s="168"/>
-      <c r="G17" s="168"/>
-      <c r="H17" s="168"/>
-      <c r="I17" s="169"/>
+      <c r="B17" s="168"/>
+      <c r="C17" s="169"/>
+      <c r="D17" s="278" t="s">
+        <v>113</v>
+      </c>
+      <c r="E17" s="279"/>
+      <c r="F17" s="279"/>
+      <c r="G17" s="279"/>
+      <c r="H17" s="279"/>
+      <c r="I17" s="280"/>
       <c r="J17" s="144" t="s">
         <v>111</v>
       </c>
       <c r="K17" s="97">
-        <v>1</v>
-      </c>
-      <c r="L17" s="154">
-        <v>325</v>
-      </c>
-      <c r="M17" s="155"/>
-      <c r="N17" s="156"/>
-      <c r="O17" s="165">
+        <v>10</v>
+      </c>
+      <c r="L17" s="273">
+        <v>242.45</v>
+      </c>
+      <c r="M17" s="274"/>
+      <c r="N17" s="275"/>
+      <c r="O17" s="173">
         <f t="shared" ref="O17:O20" si="0">K17*L17</f>
-        <v>325</v>
-      </c>
-      <c r="P17" s="165"/>
-      <c r="Q17" s="165"/>
-      <c r="R17" s="165"/>
-      <c r="S17" s="166"/>
+        <v>2424.5</v>
+      </c>
+      <c r="P17" s="173"/>
+      <c r="Q17" s="173"/>
+      <c r="R17" s="173"/>
+      <c r="S17" s="174"/>
       <c r="T17" s="127"/>
       <c r="U17" s="128"/>
       <c r="V17" s="127"/>
@@ -3744,29 +3744,29 @@
     </row>
     <row r="18" spans="1:39" s="3" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="115"/>
-      <c r="B18" s="190"/>
-      <c r="C18" s="191"/>
-      <c r="D18" s="170" t="s">
+      <c r="B18" s="160"/>
+      <c r="C18" s="161"/>
+      <c r="D18" s="281" t="s">
         <v>112</v>
       </c>
-      <c r="E18" s="171"/>
-      <c r="F18" s="171"/>
-      <c r="G18" s="171"/>
-      <c r="H18" s="171"/>
-      <c r="I18" s="172"/>
+      <c r="E18" s="282"/>
+      <c r="F18" s="282"/>
+      <c r="G18" s="282"/>
+      <c r="H18" s="282"/>
+      <c r="I18" s="283"/>
       <c r="J18" s="145"/>
       <c r="K18" s="98"/>
-      <c r="L18" s="157"/>
-      <c r="M18" s="158"/>
-      <c r="N18" s="159"/>
-      <c r="O18" s="165">
+      <c r="L18" s="170"/>
+      <c r="M18" s="171"/>
+      <c r="N18" s="172"/>
+      <c r="O18" s="173">
         <f t="shared" ref="O18:O19" si="1">K18*L18</f>
         <v>0</v>
       </c>
-      <c r="P18" s="165"/>
-      <c r="Q18" s="165"/>
-      <c r="R18" s="165"/>
-      <c r="S18" s="166"/>
+      <c r="P18" s="173"/>
+      <c r="Q18" s="173"/>
+      <c r="R18" s="173"/>
+      <c r="S18" s="174"/>
       <c r="T18" s="127"/>
       <c r="U18" s="128"/>
       <c r="V18" s="120"/>
@@ -3790,27 +3790,27 @@
     </row>
     <row r="19" spans="1:39" s="3" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="115"/>
-      <c r="B19" s="190"/>
-      <c r="C19" s="191"/>
-      <c r="D19" s="173"/>
-      <c r="E19" s="174"/>
-      <c r="F19" s="174"/>
-      <c r="G19" s="174"/>
-      <c r="H19" s="174"/>
-      <c r="I19" s="175"/>
+      <c r="B19" s="160"/>
+      <c r="C19" s="161"/>
+      <c r="D19" s="284"/>
+      <c r="E19" s="285"/>
+      <c r="F19" s="285"/>
+      <c r="G19" s="285"/>
+      <c r="H19" s="285"/>
+      <c r="I19" s="286"/>
       <c r="J19" s="145"/>
       <c r="K19" s="98"/>
-      <c r="L19" s="157"/>
-      <c r="M19" s="158"/>
-      <c r="N19" s="159"/>
-      <c r="O19" s="165">
+      <c r="L19" s="170"/>
+      <c r="M19" s="171"/>
+      <c r="N19" s="172"/>
+      <c r="O19" s="173">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P19" s="165"/>
-      <c r="Q19" s="165"/>
-      <c r="R19" s="165"/>
-      <c r="S19" s="166"/>
+      <c r="P19" s="173"/>
+      <c r="Q19" s="173"/>
+      <c r="R19" s="173"/>
+      <c r="S19" s="174"/>
       <c r="T19" s="127"/>
       <c r="U19" s="128"/>
       <c r="V19" s="120"/>
@@ -3834,8 +3834,8 @@
     </row>
     <row r="20" spans="1:39" s="3" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="115"/>
-      <c r="B20" s="190"/>
-      <c r="C20" s="191"/>
+      <c r="B20" s="160"/>
+      <c r="C20" s="161"/>
       <c r="D20" s="148"/>
       <c r="E20" s="147"/>
       <c r="F20" s="147"/>
@@ -3844,17 +3844,17 @@
       <c r="I20" s="149"/>
       <c r="J20" s="145"/>
       <c r="K20" s="98"/>
-      <c r="L20" s="157"/>
-      <c r="M20" s="158"/>
-      <c r="N20" s="159"/>
-      <c r="O20" s="165">
+      <c r="L20" s="170"/>
+      <c r="M20" s="171"/>
+      <c r="N20" s="172"/>
+      <c r="O20" s="173">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P20" s="165"/>
-      <c r="Q20" s="165"/>
-      <c r="R20" s="165"/>
-      <c r="S20" s="166"/>
+      <c r="P20" s="173"/>
+      <c r="Q20" s="173"/>
+      <c r="R20" s="173"/>
+      <c r="S20" s="174"/>
       <c r="T20" s="127"/>
       <c r="U20" s="128"/>
       <c r="V20" s="128"/>
@@ -3878,8 +3878,8 @@
     </row>
     <row r="21" spans="1:39" s="3" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="115"/>
-      <c r="B21" s="190"/>
-      <c r="C21" s="191"/>
+      <c r="B21" s="160"/>
+      <c r="C21" s="161"/>
       <c r="D21" s="148"/>
       <c r="E21" s="147"/>
       <c r="F21" s="147"/>
@@ -3888,17 +3888,17 @@
       <c r="I21" s="149"/>
       <c r="J21" s="145"/>
       <c r="K21" s="98"/>
-      <c r="L21" s="157"/>
-      <c r="M21" s="158"/>
-      <c r="N21" s="159"/>
-      <c r="O21" s="165">
+      <c r="L21" s="170"/>
+      <c r="M21" s="171"/>
+      <c r="N21" s="172"/>
+      <c r="O21" s="173">
         <f t="shared" ref="O21:O28" si="2">K21*L21</f>
         <v>0</v>
       </c>
-      <c r="P21" s="165"/>
-      <c r="Q21" s="165"/>
-      <c r="R21" s="165"/>
-      <c r="S21" s="166"/>
+      <c r="P21" s="173"/>
+      <c r="Q21" s="173"/>
+      <c r="R21" s="173"/>
+      <c r="S21" s="174"/>
       <c r="T21" s="127"/>
       <c r="U21" s="128"/>
       <c r="V21" s="128"/>
@@ -3922,8 +3922,8 @@
     </row>
     <row r="22" spans="1:39" s="3" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="115"/>
-      <c r="B22" s="190"/>
-      <c r="C22" s="191"/>
+      <c r="B22" s="160"/>
+      <c r="C22" s="161"/>
       <c r="D22" s="148"/>
       <c r="E22" s="147"/>
       <c r="F22" s="147"/>
@@ -3932,17 +3932,17 @@
       <c r="I22" s="149"/>
       <c r="J22" s="145"/>
       <c r="K22" s="98"/>
-      <c r="L22" s="157"/>
-      <c r="M22" s="158"/>
-      <c r="N22" s="159"/>
-      <c r="O22" s="165">
+      <c r="L22" s="170"/>
+      <c r="M22" s="171"/>
+      <c r="N22" s="172"/>
+      <c r="O22" s="173">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P22" s="165"/>
-      <c r="Q22" s="165"/>
-      <c r="R22" s="165"/>
-      <c r="S22" s="166"/>
+      <c r="P22" s="173"/>
+      <c r="Q22" s="173"/>
+      <c r="R22" s="173"/>
+      <c r="S22" s="174"/>
       <c r="T22" s="127"/>
       <c r="U22" s="128"/>
       <c r="V22" s="128"/>
@@ -3966,8 +3966,8 @@
     </row>
     <row r="23" spans="1:39" s="3" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="115"/>
-      <c r="B23" s="190"/>
-      <c r="C23" s="191"/>
+      <c r="B23" s="160"/>
+      <c r="C23" s="161"/>
       <c r="D23" s="148"/>
       <c r="E23" s="147"/>
       <c r="F23" s="147"/>
@@ -3976,17 +3976,17 @@
       <c r="I23" s="149"/>
       <c r="J23" s="145"/>
       <c r="K23" s="98"/>
-      <c r="L23" s="157"/>
-      <c r="M23" s="158"/>
-      <c r="N23" s="159"/>
-      <c r="O23" s="165">
+      <c r="L23" s="170"/>
+      <c r="M23" s="171"/>
+      <c r="N23" s="172"/>
+      <c r="O23" s="173">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P23" s="165"/>
-      <c r="Q23" s="165"/>
-      <c r="R23" s="165"/>
-      <c r="S23" s="166"/>
+      <c r="P23" s="173"/>
+      <c r="Q23" s="173"/>
+      <c r="R23" s="173"/>
+      <c r="S23" s="174"/>
       <c r="T23" s="127"/>
       <c r="U23" s="128"/>
       <c r="V23" s="128"/>
@@ -4010,8 +4010,8 @@
     </row>
     <row r="24" spans="1:39" s="3" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="115"/>
-      <c r="B24" s="190"/>
-      <c r="C24" s="191"/>
+      <c r="B24" s="160"/>
+      <c r="C24" s="161"/>
       <c r="D24" s="148"/>
       <c r="E24" s="147"/>
       <c r="F24" s="147"/>
@@ -4020,22 +4020,22 @@
       <c r="I24" s="149"/>
       <c r="J24" s="145"/>
       <c r="K24" s="98"/>
-      <c r="L24" s="157"/>
-      <c r="M24" s="158"/>
-      <c r="N24" s="159"/>
-      <c r="O24" s="165">
+      <c r="L24" s="170"/>
+      <c r="M24" s="171"/>
+      <c r="N24" s="172"/>
+      <c r="O24" s="173">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P24" s="165"/>
-      <c r="Q24" s="165"/>
-      <c r="R24" s="165"/>
-      <c r="S24" s="166"/>
+      <c r="P24" s="173"/>
+      <c r="Q24" s="173"/>
+      <c r="R24" s="173"/>
+      <c r="S24" s="174"/>
       <c r="T24" s="127"/>
-      <c r="U24" s="199"/>
-      <c r="V24" s="199"/>
-      <c r="W24" s="199"/>
-      <c r="X24" s="199"/>
+      <c r="U24" s="178"/>
+      <c r="V24" s="178"/>
+      <c r="W24" s="178"/>
+      <c r="X24" s="178"/>
       <c r="Y24" s="128"/>
       <c r="Z24" s="128"/>
       <c r="AA24" s="128"/>
@@ -4054,8 +4054,8 @@
     </row>
     <row r="25" spans="1:39" s="3" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="115"/>
-      <c r="B25" s="190"/>
-      <c r="C25" s="191"/>
+      <c r="B25" s="160"/>
+      <c r="C25" s="161"/>
       <c r="D25" s="148"/>
       <c r="E25" s="147"/>
       <c r="F25" s="147"/>
@@ -4064,17 +4064,17 @@
       <c r="I25" s="149"/>
       <c r="J25" s="145"/>
       <c r="K25" s="98"/>
-      <c r="L25" s="157"/>
-      <c r="M25" s="158"/>
-      <c r="N25" s="159"/>
-      <c r="O25" s="165">
+      <c r="L25" s="170"/>
+      <c r="M25" s="171"/>
+      <c r="N25" s="172"/>
+      <c r="O25" s="173">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P25" s="165"/>
-      <c r="Q25" s="165"/>
-      <c r="R25" s="165"/>
-      <c r="S25" s="166"/>
+      <c r="P25" s="173"/>
+      <c r="Q25" s="173"/>
+      <c r="R25" s="173"/>
+      <c r="S25" s="174"/>
       <c r="T25" s="127"/>
       <c r="U25" s="128"/>
       <c r="V25" s="128"/>
@@ -4098,8 +4098,8 @@
     </row>
     <row r="26" spans="1:39" s="3" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="115"/>
-      <c r="B26" s="190"/>
-      <c r="C26" s="191"/>
+      <c r="B26" s="160"/>
+      <c r="C26" s="161"/>
       <c r="D26" s="148"/>
       <c r="E26" s="147"/>
       <c r="F26" s="147"/>
@@ -4108,17 +4108,17 @@
       <c r="I26" s="149"/>
       <c r="J26" s="145"/>
       <c r="K26" s="98"/>
-      <c r="L26" s="157"/>
-      <c r="M26" s="158"/>
-      <c r="N26" s="159"/>
-      <c r="O26" s="165">
+      <c r="L26" s="170"/>
+      <c r="M26" s="171"/>
+      <c r="N26" s="172"/>
+      <c r="O26" s="173">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P26" s="165"/>
-      <c r="Q26" s="165"/>
-      <c r="R26" s="165"/>
-      <c r="S26" s="166"/>
+      <c r="P26" s="173"/>
+      <c r="Q26" s="173"/>
+      <c r="R26" s="173"/>
+      <c r="S26" s="174"/>
       <c r="T26" s="127"/>
       <c r="U26" s="128"/>
       <c r="V26" s="128"/>
@@ -4142,8 +4142,8 @@
     </row>
     <row r="27" spans="1:39" s="3" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="115"/>
-      <c r="B27" s="190"/>
-      <c r="C27" s="191"/>
+      <c r="B27" s="160"/>
+      <c r="C27" s="161"/>
       <c r="D27" s="148"/>
       <c r="E27" s="147"/>
       <c r="F27" s="147"/>
@@ -4152,17 +4152,17 @@
       <c r="I27" s="149"/>
       <c r="J27" s="145"/>
       <c r="K27" s="98"/>
-      <c r="L27" s="157"/>
-      <c r="M27" s="158"/>
-      <c r="N27" s="159"/>
-      <c r="O27" s="165">
+      <c r="L27" s="170"/>
+      <c r="M27" s="171"/>
+      <c r="N27" s="172"/>
+      <c r="O27" s="173">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P27" s="165"/>
-      <c r="Q27" s="165"/>
-      <c r="R27" s="165"/>
-      <c r="S27" s="166"/>
+      <c r="P27" s="173"/>
+      <c r="Q27" s="173"/>
+      <c r="R27" s="173"/>
+      <c r="S27" s="174"/>
       <c r="T27" s="127"/>
       <c r="U27" s="128"/>
       <c r="V27" s="128"/>
@@ -4186,8 +4186,8 @@
     </row>
     <row r="28" spans="1:39" s="3" customFormat="1" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="115"/>
-      <c r="B28" s="192"/>
-      <c r="C28" s="193"/>
+      <c r="B28" s="248"/>
+      <c r="C28" s="249"/>
       <c r="D28" s="150"/>
       <c r="E28" s="151"/>
       <c r="F28" s="151"/>
@@ -4196,17 +4196,17 @@
       <c r="I28" s="152"/>
       <c r="J28" s="146"/>
       <c r="K28" s="143"/>
-      <c r="L28" s="200"/>
-      <c r="M28" s="201"/>
-      <c r="N28" s="202"/>
-      <c r="O28" s="216">
+      <c r="L28" s="255"/>
+      <c r="M28" s="256"/>
+      <c r="N28" s="257"/>
+      <c r="O28" s="222">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P28" s="216"/>
-      <c r="Q28" s="216"/>
-      <c r="R28" s="216"/>
-      <c r="S28" s="217"/>
+      <c r="P28" s="222"/>
+      <c r="Q28" s="222"/>
+      <c r="R28" s="222"/>
+      <c r="S28" s="223"/>
       <c r="T28" s="127"/>
       <c r="U28" s="128"/>
       <c r="V28" s="128"/>
@@ -4230,31 +4230,31 @@
     </row>
     <row r="29" spans="1:39" s="3" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="115"/>
-      <c r="B29" s="194" t="s">
+      <c r="B29" s="250" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="195"/>
-      <c r="D29" s="195"/>
-      <c r="E29" s="195"/>
-      <c r="F29" s="195"/>
-      <c r="G29" s="195"/>
-      <c r="H29" s="195"/>
-      <c r="I29" s="195"/>
-      <c r="J29" s="195"/>
-      <c r="K29" s="196"/>
+      <c r="C29" s="251"/>
+      <c r="D29" s="251"/>
+      <c r="E29" s="251"/>
+      <c r="F29" s="251"/>
+      <c r="G29" s="251"/>
+      <c r="H29" s="251"/>
+      <c r="I29" s="251"/>
+      <c r="J29" s="251"/>
+      <c r="K29" s="252"/>
       <c r="L29" s="142"/>
       <c r="M29" s="140" t="s">
         <v>21</v>
       </c>
       <c r="N29" s="141"/>
-      <c r="O29" s="214">
+      <c r="O29" s="220">
         <f>SUM(O17:S28)</f>
-        <v>325</v>
-      </c>
-      <c r="P29" s="214"/>
-      <c r="Q29" s="214"/>
-      <c r="R29" s="214"/>
-      <c r="S29" s="215"/>
+        <v>2424.5</v>
+      </c>
+      <c r="P29" s="220"/>
+      <c r="Q29" s="220"/>
+      <c r="R29" s="220"/>
+      <c r="S29" s="221"/>
       <c r="T29" s="127"/>
       <c r="U29" s="128"/>
       <c r="V29" s="128"/>
@@ -4278,15 +4278,15 @@
     </row>
     <row r="30" spans="1:39" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="115"/>
-      <c r="B30" s="220" t="s">
+      <c r="B30" s="224" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="221"/>
-      <c r="D30" s="218" t="s">
+      <c r="C30" s="225"/>
+      <c r="D30" s="203" t="s">
         <v>110</v>
       </c>
-      <c r="E30" s="218"/>
-      <c r="F30" s="219"/>
+      <c r="E30" s="203"/>
+      <c r="F30" s="204"/>
       <c r="G30" s="84" t="s">
         <v>23</v>
       </c>
@@ -4294,16 +4294,18 @@
       <c r="I30" s="84"/>
       <c r="J30" s="84"/>
       <c r="K30" s="85"/>
-      <c r="L30" s="239" t="s">
+      <c r="L30" s="241" t="s">
         <v>20</v>
       </c>
-      <c r="M30" s="240"/>
-      <c r="N30" s="241"/>
-      <c r="O30" s="226"/>
-      <c r="P30" s="227"/>
-      <c r="Q30" s="227"/>
-      <c r="R30" s="227"/>
-      <c r="S30" s="228"/>
+      <c r="M30" s="242"/>
+      <c r="N30" s="243"/>
+      <c r="O30" s="228">
+        <v>160</v>
+      </c>
+      <c r="P30" s="229"/>
+      <c r="Q30" s="229"/>
+      <c r="R30" s="229"/>
+      <c r="S30" s="230"/>
       <c r="T30" s="127"/>
       <c r="U30" s="128"/>
       <c r="V30" s="128"/>
@@ -4327,33 +4329,33 @@
     </row>
     <row r="31" spans="1:39" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="115"/>
-      <c r="B31" s="222" t="s">
+      <c r="B31" s="212" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="223"/>
-      <c r="D31" s="229" t="s">
+      <c r="C31" s="213"/>
+      <c r="D31" s="231" t="s">
         <v>104</v>
       </c>
-      <c r="E31" s="229"/>
-      <c r="F31" s="230"/>
-      <c r="G31" s="231"/>
-      <c r="H31" s="232"/>
-      <c r="I31" s="232"/>
-      <c r="J31" s="232"/>
-      <c r="K31" s="233"/>
-      <c r="L31" s="257" t="s">
+      <c r="E31" s="231"/>
+      <c r="F31" s="232"/>
+      <c r="G31" s="233"/>
+      <c r="H31" s="234"/>
+      <c r="I31" s="234"/>
+      <c r="J31" s="234"/>
+      <c r="K31" s="235"/>
+      <c r="L31" s="193" t="s">
         <v>75</v>
       </c>
-      <c r="M31" s="258"/>
-      <c r="N31" s="259"/>
-      <c r="O31" s="247">
+      <c r="M31" s="194"/>
+      <c r="N31" s="195"/>
+      <c r="O31" s="183">
         <f>0.13*(O29+O30)</f>
-        <v>42.25</v>
-      </c>
-      <c r="P31" s="248"/>
-      <c r="Q31" s="248"/>
-      <c r="R31" s="248"/>
-      <c r="S31" s="249"/>
+        <v>335.98500000000001</v>
+      </c>
+      <c r="P31" s="184"/>
+      <c r="Q31" s="184"/>
+      <c r="R31" s="184"/>
+      <c r="S31" s="185"/>
       <c r="T31" s="127"/>
       <c r="U31" s="128"/>
       <c r="V31" s="128"/>
@@ -4379,22 +4381,22 @@
       <c r="A32" s="115"/>
       <c r="B32" s="133"/>
       <c r="C32" s="134"/>
-      <c r="D32" s="262"/>
-      <c r="E32" s="262"/>
-      <c r="F32" s="263"/>
-      <c r="G32" s="231"/>
-      <c r="H32" s="232"/>
-      <c r="I32" s="232"/>
-      <c r="J32" s="232"/>
-      <c r="K32" s="233"/>
-      <c r="L32" s="272"/>
-      <c r="M32" s="272"/>
-      <c r="N32" s="273"/>
-      <c r="O32" s="243"/>
-      <c r="P32" s="165"/>
-      <c r="Q32" s="165"/>
-      <c r="R32" s="165"/>
-      <c r="S32" s="166"/>
+      <c r="D32" s="198"/>
+      <c r="E32" s="198"/>
+      <c r="F32" s="199"/>
+      <c r="G32" s="233"/>
+      <c r="H32" s="234"/>
+      <c r="I32" s="234"/>
+      <c r="J32" s="234"/>
+      <c r="K32" s="235"/>
+      <c r="L32" s="210"/>
+      <c r="M32" s="210"/>
+      <c r="N32" s="211"/>
+      <c r="O32" s="179"/>
+      <c r="P32" s="173"/>
+      <c r="Q32" s="173"/>
+      <c r="R32" s="173"/>
+      <c r="S32" s="174"/>
       <c r="T32" s="127"/>
       <c r="U32" s="128"/>
       <c r="V32" s="128"/>
@@ -4418,36 +4420,36 @@
     </row>
     <row r="33" spans="1:39" s="3" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="115"/>
-      <c r="B33" s="222" t="s">
+      <c r="B33" s="212" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="223"/>
+      <c r="C33" s="213"/>
       <c r="D33" s="137"/>
       <c r="E33" s="137"/>
       <c r="F33" s="75"/>
-      <c r="G33" s="234"/>
-      <c r="H33" s="235"/>
-      <c r="I33" s="235"/>
-      <c r="J33" s="235"/>
-      <c r="K33" s="236"/>
-      <c r="L33" s="260" t="s">
+      <c r="G33" s="236"/>
+      <c r="H33" s="237"/>
+      <c r="I33" s="237"/>
+      <c r="J33" s="237"/>
+      <c r="K33" s="238"/>
+      <c r="L33" s="196" t="s">
         <v>4</v>
       </c>
-      <c r="M33" s="260"/>
-      <c r="N33" s="261"/>
-      <c r="O33" s="244">
+      <c r="M33" s="196"/>
+      <c r="N33" s="197"/>
+      <c r="O33" s="180">
         <f>O29+O30+O31</f>
-        <v>367.25</v>
-      </c>
-      <c r="P33" s="245"/>
-      <c r="Q33" s="245"/>
-      <c r="R33" s="245"/>
-      <c r="S33" s="246"/>
+        <v>2920.4850000000001</v>
+      </c>
+      <c r="P33" s="181"/>
+      <c r="Q33" s="181"/>
+      <c r="R33" s="181"/>
+      <c r="S33" s="182"/>
       <c r="T33" s="127"/>
-      <c r="U33" s="199"/>
-      <c r="V33" s="199"/>
-      <c r="W33" s="199"/>
-      <c r="X33" s="199"/>
+      <c r="U33" s="178"/>
+      <c r="V33" s="178"/>
+      <c r="W33" s="178"/>
+      <c r="X33" s="178"/>
       <c r="Y33" s="128"/>
       <c r="Z33" s="128"/>
       <c r="AA33" s="128"/>
@@ -4497,13 +4499,13 @@
     </row>
     <row r="35" spans="1:39" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="112"/>
-      <c r="B35" s="224"/>
-      <c r="C35" s="225"/>
-      <c r="D35" s="237" t="s">
+      <c r="B35" s="226"/>
+      <c r="C35" s="227"/>
+      <c r="D35" s="239" t="s">
         <v>77</v>
       </c>
-      <c r="E35" s="237"/>
-      <c r="F35" s="238"/>
+      <c r="E35" s="239"/>
+      <c r="F35" s="240"/>
       <c r="G35" s="66"/>
       <c r="H35" s="66"/>
       <c r="I35" s="83" t="s">
@@ -4542,30 +4544,30 @@
     </row>
     <row r="36" spans="1:39" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="112"/>
-      <c r="B36" s="267" t="s">
+      <c r="B36" s="205" t="s">
         <v>95</v>
       </c>
-      <c r="C36" s="268"/>
-      <c r="D36" s="212" t="s">
+      <c r="C36" s="206"/>
+      <c r="D36" s="218" t="s">
         <v>107</v>
       </c>
-      <c r="E36" s="212"/>
-      <c r="F36" s="213"/>
+      <c r="E36" s="218"/>
+      <c r="F36" s="219"/>
       <c r="G36" s="61"/>
       <c r="H36" s="61"/>
-      <c r="I36" s="269" t="s">
+      <c r="I36" s="207" t="s">
         <v>26</v>
       </c>
-      <c r="J36" s="270"/>
-      <c r="K36" s="270"/>
-      <c r="L36" s="270"/>
-      <c r="M36" s="270"/>
-      <c r="N36" s="270"/>
-      <c r="O36" s="270"/>
-      <c r="P36" s="270"/>
-      <c r="Q36" s="270"/>
-      <c r="R36" s="270"/>
-      <c r="S36" s="271"/>
+      <c r="J36" s="208"/>
+      <c r="K36" s="208"/>
+      <c r="L36" s="208"/>
+      <c r="M36" s="208"/>
+      <c r="N36" s="208"/>
+      <c r="O36" s="208"/>
+      <c r="P36" s="208"/>
+      <c r="Q36" s="208"/>
+      <c r="R36" s="208"/>
+      <c r="S36" s="209"/>
       <c r="T36" s="112"/>
       <c r="U36" s="117"/>
       <c r="V36" s="117"/>
@@ -4589,15 +4591,15 @@
     </row>
     <row r="37" spans="1:39" s="1" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="112"/>
-      <c r="B37" s="208" t="s">
+      <c r="B37" s="214" t="s">
         <v>96</v>
       </c>
-      <c r="C37" s="209"/>
-      <c r="D37" s="218">
+      <c r="C37" s="215"/>
+      <c r="D37" s="203">
         <v>2820210001</v>
       </c>
-      <c r="E37" s="218"/>
-      <c r="F37" s="219"/>
+      <c r="E37" s="203"/>
+      <c r="F37" s="204"/>
       <c r="G37" s="95"/>
       <c r="H37" s="96"/>
       <c r="I37" s="74"/>
@@ -4634,13 +4636,13 @@
     </row>
     <row r="38" spans="1:39" s="1" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="112"/>
-      <c r="B38" s="210" t="s">
+      <c r="B38" s="216" t="s">
         <v>97</v>
       </c>
-      <c r="C38" s="211"/>
-      <c r="D38" s="218"/>
-      <c r="E38" s="218"/>
-      <c r="F38" s="219"/>
+      <c r="C38" s="217"/>
+      <c r="D38" s="203"/>
+      <c r="E38" s="203"/>
+      <c r="F38" s="204"/>
       <c r="G38" s="61"/>
       <c r="H38" s="61"/>
       <c r="I38" s="61"/>
@@ -4718,26 +4720,26 @@
     </row>
     <row r="40" spans="1:39" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="112"/>
-      <c r="B40" s="264" t="s">
+      <c r="B40" s="200" t="s">
         <v>99</v>
       </c>
-      <c r="C40" s="265"/>
-      <c r="D40" s="265"/>
-      <c r="E40" s="265"/>
-      <c r="F40" s="265"/>
-      <c r="G40" s="265"/>
-      <c r="H40" s="265"/>
-      <c r="I40" s="265"/>
-      <c r="J40" s="265"/>
-      <c r="K40" s="265"/>
-      <c r="L40" s="265"/>
-      <c r="M40" s="265"/>
-      <c r="N40" s="265"/>
-      <c r="O40" s="265"/>
-      <c r="P40" s="265"/>
-      <c r="Q40" s="265"/>
-      <c r="R40" s="265"/>
-      <c r="S40" s="266"/>
+      <c r="C40" s="201"/>
+      <c r="D40" s="201"/>
+      <c r="E40" s="201"/>
+      <c r="F40" s="201"/>
+      <c r="G40" s="201"/>
+      <c r="H40" s="201"/>
+      <c r="I40" s="201"/>
+      <c r="J40" s="201"/>
+      <c r="K40" s="201"/>
+      <c r="L40" s="201"/>
+      <c r="M40" s="201"/>
+      <c r="N40" s="201"/>
+      <c r="O40" s="201"/>
+      <c r="P40" s="201"/>
+      <c r="Q40" s="201"/>
+      <c r="R40" s="201"/>
+      <c r="S40" s="202"/>
       <c r="T40" s="117"/>
       <c r="U40" s="117"/>
       <c r="V40" s="117"/>
@@ -5012,25 +5014,25 @@
     </row>
     <row r="48" spans="1:39" s="1" customFormat="1" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="112"/>
-      <c r="B48" s="255" t="s">
+      <c r="B48" s="191" t="s">
         <v>3</v>
       </c>
-      <c r="C48" s="255"/>
-      <c r="D48" s="255"/>
-      <c r="E48" s="255"/>
-      <c r="F48" s="255"/>
-      <c r="G48" s="255"/>
-      <c r="H48" s="255"/>
-      <c r="I48" s="255"/>
-      <c r="J48" s="255"/>
-      <c r="K48" s="255"/>
-      <c r="L48" s="255"/>
-      <c r="M48" s="255"/>
-      <c r="N48" s="255"/>
-      <c r="O48" s="255"/>
-      <c r="P48" s="255"/>
-      <c r="Q48" s="255"/>
-      <c r="R48" s="255"/>
+      <c r="C48" s="191"/>
+      <c r="D48" s="191"/>
+      <c r="E48" s="191"/>
+      <c r="F48" s="191"/>
+      <c r="G48" s="191"/>
+      <c r="H48" s="191"/>
+      <c r="I48" s="191"/>
+      <c r="J48" s="191"/>
+      <c r="K48" s="191"/>
+      <c r="L48" s="191"/>
+      <c r="M48" s="191"/>
+      <c r="N48" s="191"/>
+      <c r="O48" s="191"/>
+      <c r="P48" s="191"/>
+      <c r="Q48" s="191"/>
+      <c r="R48" s="191"/>
       <c r="T48" s="112"/>
       <c r="U48" s="117"/>
       <c r="V48" s="117"/>
@@ -5054,23 +5056,23 @@
     </row>
     <row r="49" spans="1:39" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="112"/>
-      <c r="B49" s="255"/>
-      <c r="C49" s="255"/>
-      <c r="D49" s="255"/>
-      <c r="E49" s="255"/>
-      <c r="F49" s="255"/>
-      <c r="G49" s="255"/>
-      <c r="H49" s="255"/>
-      <c r="I49" s="255"/>
-      <c r="J49" s="255"/>
-      <c r="K49" s="255"/>
-      <c r="L49" s="255"/>
-      <c r="M49" s="255"/>
-      <c r="N49" s="255"/>
-      <c r="O49" s="255"/>
-      <c r="P49" s="255"/>
-      <c r="Q49" s="255"/>
-      <c r="R49" s="255"/>
+      <c r="B49" s="191"/>
+      <c r="C49" s="191"/>
+      <c r="D49" s="191"/>
+      <c r="E49" s="191"/>
+      <c r="F49" s="191"/>
+      <c r="G49" s="191"/>
+      <c r="H49" s="191"/>
+      <c r="I49" s="191"/>
+      <c r="J49" s="191"/>
+      <c r="K49" s="191"/>
+      <c r="L49" s="191"/>
+      <c r="M49" s="191"/>
+      <c r="N49" s="191"/>
+      <c r="O49" s="191"/>
+      <c r="P49" s="191"/>
+      <c r="Q49" s="191"/>
+      <c r="R49" s="191"/>
       <c r="T49" s="112"/>
       <c r="U49" s="117"/>
       <c r="V49" s="117"/>
@@ -5137,23 +5139,23 @@
       <c r="C51" s="51">
         <v>1</v>
       </c>
-      <c r="D51" s="256" t="s">
+      <c r="D51" s="192" t="s">
         <v>7</v>
       </c>
-      <c r="E51" s="256"/>
-      <c r="F51" s="256"/>
-      <c r="G51" s="256"/>
-      <c r="H51" s="256"/>
-      <c r="I51" s="256"/>
-      <c r="J51" s="256"/>
-      <c r="K51" s="256"/>
-      <c r="L51" s="256"/>
-      <c r="M51" s="256"/>
-      <c r="N51" s="256"/>
-      <c r="O51" s="256"/>
-      <c r="P51" s="256"/>
-      <c r="Q51" s="256"/>
-      <c r="R51" s="256"/>
+      <c r="E51" s="192"/>
+      <c r="F51" s="192"/>
+      <c r="G51" s="192"/>
+      <c r="H51" s="192"/>
+      <c r="I51" s="192"/>
+      <c r="J51" s="192"/>
+      <c r="K51" s="192"/>
+      <c r="L51" s="192"/>
+      <c r="M51" s="192"/>
+      <c r="N51" s="192"/>
+      <c r="O51" s="192"/>
+      <c r="P51" s="192"/>
+      <c r="Q51" s="192"/>
+      <c r="R51" s="192"/>
       <c r="T51" s="112"/>
       <c r="U51" s="117"/>
       <c r="V51" s="117"/>
@@ -5219,23 +5221,23 @@
       <c r="C53" s="59">
         <v>2</v>
       </c>
-      <c r="D53" s="251" t="s">
+      <c r="D53" s="187" t="s">
         <v>16</v>
       </c>
-      <c r="E53" s="251"/>
-      <c r="F53" s="251"/>
-      <c r="G53" s="251"/>
-      <c r="H53" s="251"/>
-      <c r="I53" s="251"/>
-      <c r="J53" s="251"/>
-      <c r="K53" s="251"/>
-      <c r="L53" s="251"/>
-      <c r="M53" s="251"/>
-      <c r="N53" s="251"/>
-      <c r="O53" s="251"/>
-      <c r="P53" s="251"/>
-      <c r="Q53" s="251"/>
-      <c r="R53" s="251"/>
+      <c r="E53" s="187"/>
+      <c r="F53" s="187"/>
+      <c r="G53" s="187"/>
+      <c r="H53" s="187"/>
+      <c r="I53" s="187"/>
+      <c r="J53" s="187"/>
+      <c r="K53" s="187"/>
+      <c r="L53" s="187"/>
+      <c r="M53" s="187"/>
+      <c r="N53" s="187"/>
+      <c r="O53" s="187"/>
+      <c r="P53" s="187"/>
+      <c r="Q53" s="187"/>
+      <c r="R53" s="187"/>
       <c r="T53" s="112"/>
       <c r="U53" s="117"/>
       <c r="V53" s="117"/>
@@ -5301,23 +5303,23 @@
       <c r="C55" s="51">
         <v>3</v>
       </c>
-      <c r="D55" s="251" t="s">
+      <c r="D55" s="187" t="s">
         <v>9</v>
       </c>
-      <c r="E55" s="251"/>
-      <c r="F55" s="251"/>
-      <c r="G55" s="251"/>
-      <c r="H55" s="251"/>
-      <c r="I55" s="251"/>
-      <c r="J55" s="251"/>
-      <c r="K55" s="251"/>
-      <c r="L55" s="251"/>
-      <c r="M55" s="251"/>
-      <c r="N55" s="251"/>
-      <c r="O55" s="251"/>
-      <c r="P55" s="251"/>
-      <c r="Q55" s="251"/>
-      <c r="R55" s="251"/>
+      <c r="E55" s="187"/>
+      <c r="F55" s="187"/>
+      <c r="G55" s="187"/>
+      <c r="H55" s="187"/>
+      <c r="I55" s="187"/>
+      <c r="J55" s="187"/>
+      <c r="K55" s="187"/>
+      <c r="L55" s="187"/>
+      <c r="M55" s="187"/>
+      <c r="N55" s="187"/>
+      <c r="O55" s="187"/>
+      <c r="P55" s="187"/>
+      <c r="Q55" s="187"/>
+      <c r="R55" s="187"/>
       <c r="T55" s="112"/>
       <c r="U55" s="117"/>
       <c r="V55" s="117"/>
@@ -5342,10 +5344,10 @@
     <row r="56" spans="1:39" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A56" s="112"/>
       <c r="C56" s="51"/>
-      <c r="D56" s="252"/>
-      <c r="E56" s="252"/>
-      <c r="F56" s="253"/>
-      <c r="G56" s="253"/>
+      <c r="D56" s="188"/>
+      <c r="E56" s="188"/>
+      <c r="F56" s="189"/>
+      <c r="G56" s="189"/>
       <c r="H56" s="57"/>
       <c r="I56" s="57"/>
       <c r="J56" s="57"/>
@@ -5383,23 +5385,23 @@
       <c r="C57" s="51">
         <v>4</v>
       </c>
-      <c r="D57" s="250" t="s">
+      <c r="D57" s="186" t="s">
         <v>17</v>
       </c>
-      <c r="E57" s="250"/>
-      <c r="F57" s="250"/>
-      <c r="G57" s="250"/>
-      <c r="H57" s="250"/>
-      <c r="I57" s="250"/>
-      <c r="J57" s="250"/>
-      <c r="K57" s="250"/>
-      <c r="L57" s="250"/>
-      <c r="M57" s="250"/>
-      <c r="N57" s="250"/>
-      <c r="O57" s="250"/>
-      <c r="P57" s="250"/>
-      <c r="Q57" s="250"/>
-      <c r="R57" s="250"/>
+      <c r="E57" s="186"/>
+      <c r="F57" s="186"/>
+      <c r="G57" s="186"/>
+      <c r="H57" s="186"/>
+      <c r="I57" s="186"/>
+      <c r="J57" s="186"/>
+      <c r="K57" s="186"/>
+      <c r="L57" s="186"/>
+      <c r="M57" s="186"/>
+      <c r="N57" s="186"/>
+      <c r="O57" s="186"/>
+      <c r="P57" s="186"/>
+      <c r="Q57" s="186"/>
+      <c r="R57" s="186"/>
       <c r="T57" s="112"/>
       <c r="U57" s="117"/>
       <c r="V57" s="117"/>
@@ -5424,21 +5426,21 @@
     <row r="58" spans="1:39" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A58" s="112"/>
       <c r="C58" s="51"/>
-      <c r="D58" s="254"/>
-      <c r="E58" s="254"/>
-      <c r="F58" s="254"/>
-      <c r="G58" s="254"/>
-      <c r="H58" s="254"/>
-      <c r="I58" s="254"/>
-      <c r="J58" s="254"/>
-      <c r="K58" s="254"/>
-      <c r="L58" s="254"/>
-      <c r="M58" s="254"/>
-      <c r="N58" s="254"/>
-      <c r="O58" s="254"/>
-      <c r="P58" s="254"/>
-      <c r="Q58" s="254"/>
-      <c r="R58" s="254"/>
+      <c r="D58" s="190"/>
+      <c r="E58" s="190"/>
+      <c r="F58" s="190"/>
+      <c r="G58" s="190"/>
+      <c r="H58" s="190"/>
+      <c r="I58" s="190"/>
+      <c r="J58" s="190"/>
+      <c r="K58" s="190"/>
+      <c r="L58" s="190"/>
+      <c r="M58" s="190"/>
+      <c r="N58" s="190"/>
+      <c r="O58" s="190"/>
+      <c r="P58" s="190"/>
+      <c r="Q58" s="190"/>
+      <c r="R58" s="190"/>
       <c r="T58" s="112"/>
       <c r="U58" s="117"/>
       <c r="V58" s="117"/>
@@ -5465,21 +5467,21 @@
       <c r="C59" s="51">
         <v>5</v>
       </c>
-      <c r="D59" s="250" t="s">
+      <c r="D59" s="186" t="s">
         <v>27</v>
       </c>
-      <c r="E59" s="250"/>
-      <c r="F59" s="250"/>
-      <c r="G59" s="250"/>
-      <c r="H59" s="250"/>
-      <c r="I59" s="250"/>
-      <c r="J59" s="250"/>
-      <c r="K59" s="250"/>
-      <c r="L59" s="250"/>
-      <c r="M59" s="250"/>
-      <c r="N59" s="250"/>
-      <c r="O59" s="250"/>
-      <c r="P59" s="250"/>
+      <c r="E59" s="186"/>
+      <c r="F59" s="186"/>
+      <c r="G59" s="186"/>
+      <c r="H59" s="186"/>
+      <c r="I59" s="186"/>
+      <c r="J59" s="186"/>
+      <c r="K59" s="186"/>
+      <c r="L59" s="186"/>
+      <c r="M59" s="186"/>
+      <c r="N59" s="186"/>
+      <c r="O59" s="186"/>
+      <c r="P59" s="186"/>
       <c r="Q59" s="56"/>
       <c r="R59" s="56"/>
       <c r="T59" s="112"/>
@@ -5506,21 +5508,21 @@
     <row r="60" spans="1:39" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="112"/>
       <c r="C60" s="51"/>
-      <c r="D60" s="251" t="s">
+      <c r="D60" s="187" t="s">
         <v>29</v>
       </c>
-      <c r="E60" s="251"/>
-      <c r="F60" s="251"/>
-      <c r="G60" s="251"/>
-      <c r="H60" s="251"/>
-      <c r="I60" s="251"/>
-      <c r="J60" s="251"/>
-      <c r="K60" s="251"/>
-      <c r="L60" s="251"/>
-      <c r="M60" s="251"/>
-      <c r="N60" s="251"/>
-      <c r="O60" s="251"/>
-      <c r="P60" s="251"/>
+      <c r="E60" s="187"/>
+      <c r="F60" s="187"/>
+      <c r="G60" s="187"/>
+      <c r="H60" s="187"/>
+      <c r="I60" s="187"/>
+      <c r="J60" s="187"/>
+      <c r="K60" s="187"/>
+      <c r="L60" s="187"/>
+      <c r="M60" s="187"/>
+      <c r="N60" s="187"/>
+      <c r="O60" s="187"/>
+      <c r="P60" s="187"/>
       <c r="Q60" s="56"/>
       <c r="R60" s="56"/>
       <c r="T60" s="112"/>
@@ -5731,18 +5733,18 @@
     </row>
     <row r="66" spans="1:39" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="117"/>
-      <c r="B66" s="242" t="s">
+      <c r="B66" s="177" t="s">
         <v>45</v>
       </c>
-      <c r="C66" s="242"/>
-      <c r="D66" s="242"/>
-      <c r="E66" s="242"/>
-      <c r="F66" s="242"/>
-      <c r="G66" s="242"/>
-      <c r="H66" s="242"/>
-      <c r="I66" s="242"/>
-      <c r="J66" s="242"/>
-      <c r="K66" s="242"/>
+      <c r="C66" s="177"/>
+      <c r="D66" s="177"/>
+      <c r="E66" s="177"/>
+      <c r="F66" s="177"/>
+      <c r="G66" s="177"/>
+      <c r="H66" s="177"/>
+      <c r="I66" s="177"/>
+      <c r="J66" s="177"/>
+      <c r="K66" s="177"/>
       <c r="L66" s="11"/>
       <c r="N66" s="16"/>
       <c r="O66" s="15"/>
@@ -6210,6 +6212,97 @@
     </row>
   </sheetData>
   <mergeCells count="115">
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="L18:N18"/>
+    <mergeCell ref="D16:I16"/>
+    <mergeCell ref="L19:N19"/>
+    <mergeCell ref="O16:S16"/>
+    <mergeCell ref="O17:S17"/>
+    <mergeCell ref="O18:S18"/>
+    <mergeCell ref="O19:S19"/>
+    <mergeCell ref="D17:I17"/>
+    <mergeCell ref="D18:I18"/>
+    <mergeCell ref="D19:I19"/>
+    <mergeCell ref="M3:S3"/>
+    <mergeCell ref="M4:S4"/>
+    <mergeCell ref="M5:R5"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="W8:W10"/>
+    <mergeCell ref="L7:S7"/>
+    <mergeCell ref="L8:S8"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="Y4:Y5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="W4:W5"/>
+    <mergeCell ref="X4:X5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:K29"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="O25:S25"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="L28:N28"/>
+    <mergeCell ref="X8:X10"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="L12:S12"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="O24:S24"/>
+    <mergeCell ref="L24:N24"/>
+    <mergeCell ref="L25:N25"/>
+    <mergeCell ref="L26:N26"/>
+    <mergeCell ref="O22:S22"/>
+    <mergeCell ref="O23:S23"/>
+    <mergeCell ref="L23:N23"/>
+    <mergeCell ref="O26:S26"/>
+    <mergeCell ref="O27:S27"/>
+    <mergeCell ref="O29:S29"/>
+    <mergeCell ref="O28:S28"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="O30:S30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="G31:K33"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="L30:N30"/>
+    <mergeCell ref="B66:K66"/>
+    <mergeCell ref="U33:X33"/>
+    <mergeCell ref="O32:S32"/>
+    <mergeCell ref="O33:S33"/>
+    <mergeCell ref="O31:S31"/>
+    <mergeCell ref="D59:P59"/>
+    <mergeCell ref="D60:P60"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="D57:R57"/>
+    <mergeCell ref="D58:R58"/>
+    <mergeCell ref="D55:R55"/>
+    <mergeCell ref="B48:R49"/>
+    <mergeCell ref="D51:R51"/>
+    <mergeCell ref="L31:N31"/>
+    <mergeCell ref="L33:N33"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D53:R53"/>
+    <mergeCell ref="B40:S40"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="I36:S36"/>
+    <mergeCell ref="L32:N32"/>
+    <mergeCell ref="B31:C31"/>
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="F3:K3"/>
     <mergeCell ref="F4:K4"/>
@@ -6234,97 +6327,6 @@
     <mergeCell ref="L14:S14"/>
     <mergeCell ref="L11:S11"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B66:K66"/>
-    <mergeCell ref="U33:X33"/>
-    <mergeCell ref="O32:S32"/>
-    <mergeCell ref="O33:S33"/>
-    <mergeCell ref="O31:S31"/>
-    <mergeCell ref="D59:P59"/>
-    <mergeCell ref="D60:P60"/>
-    <mergeCell ref="D56:G56"/>
-    <mergeCell ref="D57:R57"/>
-    <mergeCell ref="D58:R58"/>
-    <mergeCell ref="D55:R55"/>
-    <mergeCell ref="B48:R49"/>
-    <mergeCell ref="D51:R51"/>
-    <mergeCell ref="L31:N31"/>
-    <mergeCell ref="L33:N33"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D53:R53"/>
-    <mergeCell ref="B40:S40"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="I36:S36"/>
-    <mergeCell ref="L32:N32"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="O24:S24"/>
-    <mergeCell ref="L24:N24"/>
-    <mergeCell ref="L25:N25"/>
-    <mergeCell ref="L26:N26"/>
-    <mergeCell ref="O22:S22"/>
-    <mergeCell ref="O23:S23"/>
-    <mergeCell ref="L23:N23"/>
-    <mergeCell ref="O26:S26"/>
-    <mergeCell ref="O27:S27"/>
-    <mergeCell ref="O29:S29"/>
-    <mergeCell ref="O28:S28"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="O30:S30"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="G31:K33"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="L30:N30"/>
-    <mergeCell ref="Y4:Y5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="W4:W5"/>
-    <mergeCell ref="X4:X5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:K29"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="U24:X24"/>
-    <mergeCell ref="O25:S25"/>
-    <mergeCell ref="L27:N27"/>
-    <mergeCell ref="L28:N28"/>
-    <mergeCell ref="X8:X10"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="L12:S12"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="L16:N16"/>
-    <mergeCell ref="M3:S3"/>
-    <mergeCell ref="M4:S4"/>
-    <mergeCell ref="M5:R5"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="W8:W10"/>
-    <mergeCell ref="L7:S7"/>
-    <mergeCell ref="L8:S8"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="L17:N17"/>
-    <mergeCell ref="L18:N18"/>
-    <mergeCell ref="D16:I16"/>
-    <mergeCell ref="L19:N19"/>
-    <mergeCell ref="O16:S16"/>
-    <mergeCell ref="O17:S17"/>
-    <mergeCell ref="O18:S18"/>
-    <mergeCell ref="O19:S19"/>
-    <mergeCell ref="D17:I17"/>
-    <mergeCell ref="D18:I18"/>
-    <mergeCell ref="D19:I19"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations disablePrompts="1" count="2">
@@ -6796,159 +6798,159 @@
       <c r="A23" s="5"/>
       <c r="B23" s="40"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="252" t="s">
+      <c r="D23" s="188" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="252"/>
-      <c r="F23" s="252"/>
-      <c r="G23" s="252"/>
-      <c r="H23" s="252"/>
-      <c r="I23" s="252"/>
-      <c r="J23" s="252"/>
-      <c r="K23" s="252"/>
-      <c r="L23" s="252"/>
-      <c r="M23" s="252"/>
-      <c r="N23" s="252"/>
-      <c r="O23" s="252"/>
+      <c r="E23" s="188"/>
+      <c r="F23" s="188"/>
+      <c r="G23" s="188"/>
+      <c r="H23" s="188"/>
+      <c r="I23" s="188"/>
+      <c r="J23" s="188"/>
+      <c r="K23" s="188"/>
+      <c r="L23" s="188"/>
+      <c r="M23" s="188"/>
+      <c r="N23" s="188"/>
+      <c r="O23" s="188"/>
       <c r="P23" s="9"/>
     </row>
     <row r="24" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="40"/>
       <c r="C24" s="5"/>
-      <c r="D24" s="252" t="s">
+      <c r="D24" s="188" t="s">
         <v>46</v>
       </c>
-      <c r="E24" s="252"/>
-      <c r="F24" s="252"/>
-      <c r="G24" s="252"/>
-      <c r="H24" s="252"/>
-      <c r="I24" s="252"/>
-      <c r="J24" s="252"/>
-      <c r="K24" s="252"/>
-      <c r="L24" s="252"/>
-      <c r="M24" s="252"/>
-      <c r="N24" s="252"/>
-      <c r="O24" s="252"/>
+      <c r="E24" s="188"/>
+      <c r="F24" s="188"/>
+      <c r="G24" s="188"/>
+      <c r="H24" s="188"/>
+      <c r="I24" s="188"/>
+      <c r="J24" s="188"/>
+      <c r="K24" s="188"/>
+      <c r="L24" s="188"/>
+      <c r="M24" s="188"/>
+      <c r="N24" s="188"/>
+      <c r="O24" s="188"/>
       <c r="P24" s="9"/>
     </row>
     <row r="25" spans="1:16" s="39" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="41"/>
       <c r="C25" s="12"/>
-      <c r="D25" s="252" t="s">
+      <c r="D25" s="188" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="252"/>
-      <c r="F25" s="252"/>
-      <c r="G25" s="252"/>
-      <c r="H25" s="252"/>
-      <c r="I25" s="252"/>
-      <c r="J25" s="252"/>
-      <c r="K25" s="252"/>
-      <c r="L25" s="252"/>
-      <c r="M25" s="252"/>
-      <c r="N25" s="252"/>
-      <c r="O25" s="252"/>
+      <c r="E25" s="188"/>
+      <c r="F25" s="188"/>
+      <c r="G25" s="188"/>
+      <c r="H25" s="188"/>
+      <c r="I25" s="188"/>
+      <c r="J25" s="188"/>
+      <c r="K25" s="188"/>
+      <c r="L25" s="188"/>
+      <c r="M25" s="188"/>
+      <c r="N25" s="188"/>
+      <c r="O25" s="188"/>
       <c r="P25" s="13"/>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="40"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="252" t="s">
+      <c r="D26" s="188" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="252"/>
-      <c r="F26" s="252"/>
-      <c r="G26" s="252"/>
-      <c r="H26" s="252"/>
-      <c r="I26" s="252"/>
-      <c r="J26" s="252"/>
-      <c r="K26" s="252"/>
-      <c r="L26" s="252"/>
-      <c r="M26" s="252"/>
-      <c r="N26" s="252"/>
-      <c r="O26" s="252"/>
+      <c r="E26" s="188"/>
+      <c r="F26" s="188"/>
+      <c r="G26" s="188"/>
+      <c r="H26" s="188"/>
+      <c r="I26" s="188"/>
+      <c r="J26" s="188"/>
+      <c r="K26" s="188"/>
+      <c r="L26" s="188"/>
+      <c r="M26" s="188"/>
+      <c r="N26" s="188"/>
+      <c r="O26" s="188"/>
       <c r="P26" s="9"/>
     </row>
     <row r="27" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="40"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="252" t="s">
+      <c r="D27" s="188" t="s">
         <v>39</v>
       </c>
-      <c r="E27" s="252"/>
-      <c r="F27" s="252"/>
-      <c r="G27" s="252"/>
-      <c r="H27" s="252"/>
-      <c r="I27" s="252"/>
-      <c r="J27" s="252"/>
-      <c r="K27" s="252"/>
-      <c r="L27" s="252"/>
-      <c r="M27" s="252"/>
-      <c r="N27" s="252"/>
-      <c r="O27" s="252"/>
+      <c r="E27" s="188"/>
+      <c r="F27" s="188"/>
+      <c r="G27" s="188"/>
+      <c r="H27" s="188"/>
+      <c r="I27" s="188"/>
+      <c r="J27" s="188"/>
+      <c r="K27" s="188"/>
+      <c r="L27" s="188"/>
+      <c r="M27" s="188"/>
+      <c r="N27" s="188"/>
+      <c r="O27" s="188"/>
     </row>
     <row r="28" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="40"/>
       <c r="C28" s="5"/>
-      <c r="D28" s="252" t="s">
+      <c r="D28" s="188" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="252"/>
-      <c r="F28" s="252"/>
-      <c r="G28" s="252"/>
-      <c r="H28" s="252"/>
-      <c r="I28" s="252"/>
-      <c r="J28" s="252"/>
-      <c r="K28" s="252"/>
-      <c r="L28" s="252"/>
-      <c r="M28" s="252"/>
-      <c r="N28" s="252"/>
-      <c r="O28" s="252"/>
+      <c r="E28" s="188"/>
+      <c r="F28" s="188"/>
+      <c r="G28" s="188"/>
+      <c r="H28" s="188"/>
+      <c r="I28" s="188"/>
+      <c r="J28" s="188"/>
+      <c r="K28" s="188"/>
+      <c r="L28" s="188"/>
+      <c r="M28" s="188"/>
+      <c r="N28" s="188"/>
+      <c r="O28" s="188"/>
       <c r="P28" s="9"/>
     </row>
     <row r="29" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="40"/>
       <c r="C29" s="5"/>
-      <c r="D29" s="252" t="s">
+      <c r="D29" s="188" t="s">
         <v>41</v>
       </c>
-      <c r="E29" s="252"/>
-      <c r="F29" s="252"/>
-      <c r="G29" s="252"/>
-      <c r="H29" s="252"/>
-      <c r="I29" s="252"/>
-      <c r="J29" s="252"/>
-      <c r="K29" s="252"/>
-      <c r="L29" s="252"/>
-      <c r="M29" s="252"/>
-      <c r="N29" s="252"/>
-      <c r="O29" s="252"/>
+      <c r="E29" s="188"/>
+      <c r="F29" s="188"/>
+      <c r="G29" s="188"/>
+      <c r="H29" s="188"/>
+      <c r="I29" s="188"/>
+      <c r="J29" s="188"/>
+      <c r="K29" s="188"/>
+      <c r="L29" s="188"/>
+      <c r="M29" s="188"/>
+      <c r="N29" s="188"/>
+      <c r="O29" s="188"/>
       <c r="P29" s="9"/>
     </row>
     <row r="30" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="40"/>
       <c r="C30" s="5"/>
-      <c r="D30" s="252" t="s">
+      <c r="D30" s="188" t="s">
         <v>42</v>
       </c>
-      <c r="E30" s="252"/>
-      <c r="F30" s="252"/>
-      <c r="G30" s="252"/>
-      <c r="H30" s="252"/>
-      <c r="I30" s="252"/>
-      <c r="J30" s="252"/>
-      <c r="K30" s="252"/>
-      <c r="L30" s="252"/>
-      <c r="M30" s="252"/>
-      <c r="N30" s="252"/>
-      <c r="O30" s="252"/>
+      <c r="E30" s="188"/>
+      <c r="F30" s="188"/>
+      <c r="G30" s="188"/>
+      <c r="H30" s="188"/>
+      <c r="I30" s="188"/>
+      <c r="J30" s="188"/>
+      <c r="K30" s="188"/>
+      <c r="L30" s="188"/>
+      <c r="M30" s="188"/>
+      <c r="N30" s="188"/>
+      <c r="O30" s="188"/>
       <c r="P30" s="9"/>
     </row>
     <row r="31" spans="1:16" s="39" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>